<commit_message>
importo productos gope en tabla productos
</commit_message>
<xml_diff>
--- a/resources/external_files/PRECIOS-IVSOM-2018-2019 (1) - copia.xlsx
+++ b/resources/external_files/PRECIOS-IVSOM-2018-2019 (1) - copia.xlsx
@@ -2904,15 +2904,15 @@
   </sheetPr>
   <dimension ref="A1:H314"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.8097165991903"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.2348178137652"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6032388663968"/>

</xml_diff>